<commit_message>
Stat descriptive du fichier tableau parcelle
</commit_message>
<xml_diff>
--- a/TableauxdonnéesParcelle.xlsx
+++ b/TableauxdonnéesParcelle.xlsx
@@ -584,16 +584,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,10 +615,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="O34" activeCellId="0" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="970" style="0" width="12.83"/>
   </cols>
@@ -864,7 +860,7 @@
       <c r="D8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -1882,7 +1878,7 @@
       <c r="B40" s="0" t="n">
         <v>2023</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="0" t="s">
@@ -1914,7 +1910,7 @@
       <c r="B41" s="0" t="n">
         <v>2023</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="0" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="0" t="s">
@@ -3546,7 +3542,7 @@
       <c r="B92" s="0" t="n">
         <v>2023</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="0" t="s">
         <v>58</v>
       </c>
       <c r="D92" s="0" t="s">
@@ -3578,7 +3574,7 @@
       <c r="B93" s="0" t="n">
         <v>2023</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="0" t="s">
         <v>58</v>
       </c>
       <c r="D93" s="0" t="s">

</xml_diff>